<commit_message>
updated overlay and spreadsheet based on EA feedback.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-oracle-java-runtime-environment-7-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-oracle-java-runtime-environment-7-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-oracle-java-runtime-environment-7-unix-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DAF305AE-CC27-4E9C-A47B-DAFA575B8406}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4F320476-3C37-6742-9130-720207F5651B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-oracle-jav" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="84" uniqueCount="70">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="84" uniqueCount="71">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -381,13 +381,66 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CCI-001162
+The organization establishes implementation guidance for acceptable mobile code and mobile code technologies.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">SC-18
-</t>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NIST SP 800-53::SC-18
+NIST SP 800-53A::SC-18
+NIST SP 800-53 Revision 4::SC-18
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001695
+The information system prevents the execution of organization-defined unacceptable mobile code.
+NIST SP 800-53 :: SC-18 (3)
+NIST SP 800-53A :: SC-18 (3).1
+NIST SP 800-53 Revision 4 :: SC-18 (3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CCI-001162
+The organization establishes implementation guidance for acceptable mobile code and mobile code technologies.
+NIST SP 800-53::SC-18
+NIST SP 800-53A::SC-18
+NIST SP 800-53 Revision 4::SC-18</t>
     </r>
   </si>
 </sst>
@@ -395,7 +448,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,6 +590,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="34">
@@ -918,10 +976,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1283,22 +1341,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.84765625" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="45" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="51.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="53" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1484375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.84765625" style="1"/>
+    <col min="7" max="7" width="24.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1379,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="218.4" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:7" ht="388">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1340,11 +1398,11 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="296.39999999999998" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:7" ht="356">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1363,12 +1421,12 @@
       <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>69</v>
+      <c r="G3" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="218.4" x14ac:dyDescent="0.6">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:7" ht="238">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1390,8 +1448,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="249.6" x14ac:dyDescent="0.6">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:7" ht="272">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1413,8 +1471,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="218.4" x14ac:dyDescent="0.6">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:7" ht="272">
+      <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1436,8 +1494,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="265.2" x14ac:dyDescent="0.6">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:7" ht="306">
+      <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1459,8 +1517,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="187.2" x14ac:dyDescent="0.6">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:7" ht="204">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1482,8 +1540,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="156" x14ac:dyDescent="0.6">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:7" ht="170">
+      <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1505,8 +1563,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="202.8" x14ac:dyDescent="0.6">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:7" ht="221">
+      <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1528,8 +1586,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="171.6" x14ac:dyDescent="0.6">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:7" ht="221">
+      <c r="A11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1551,8 +1609,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="171.6" x14ac:dyDescent="0.6">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:7" ht="187">
+      <c r="A12" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="5" t="s">

</xml_diff>